<commit_message>
created function in while.py using input
</commit_message>
<xml_diff>
--- a/olx_products.xlsx
+++ b/olx_products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,27 +466,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>СКИДКА до 01.09.22!Беспроводная мышка Razer Deathadder V2 X Hyperspeed</t>
+          <t>GSM репитер Сотовая связь 4г, gsm aloqa internet 4G, усилитель сигнала</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.olx.uz/d/oz/obyavlenie/skidka-do-01-09-22-besprovodnaya-myshka-razer-deathadder-v2-x-hyperspeed-ID26NPB.html</t>
+          <t>https://www.olx.uz/d/oz/obyavlenie/gsm-repiter-sotovaya-svyaz-4g-gsm-aloqa-internet-4g-usilitel-signala-ID2bWxM.html</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>70 у.е.</t>
+          <t>99 у.е.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Toshkent, Yakkasaroy tumani - 10-avgust, 2022</t>
+          <t>Toshkent, Olmazor tumani - Bugunda 05:36</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10-avgust, 2022</t>
+          <t>Bugunda 05:36</t>
         </is>
       </c>
     </row>
@@ -496,27 +496,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Shipadoo клавятура</t>
+          <t>СКИДКА до 05.09!Беспроводной Джойстик Компьютер,PS3,Телефон Sven 5070</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.olx.uz/d/oz/obyavlenie/shipadoo-klavyatura-ID2XRgx.html</t>
+          <t>https://www.olx.uz/d/oz/obyavlenie/skidka-do-05-09-besprovodnoj-dzhojstik-kompyuter-ps3-telefon-sven-5070-ID2xSWA.html</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>200 000 so’m</t>
+          <t>35 у.е.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Navoiy - 24-avgust, 2022</t>
+          <t>Toshkent, Yakkasaroy tumani - 30-avgust, 2022</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>24-avgust, 2022</t>
+          <t>30-avgust, 2022</t>
         </is>
       </c>
     </row>
@@ -526,27 +526,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>СКИДКА!Док Станция+Беспроводная мышка RAZER Viper Ultimate Cyberpunk</t>
+          <t>TP-Link Archer AX55 AX3000 Двухдиапазонный гигабитный Wi‑Fi 6 роутер.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.olx.uz/d/oz/obyavlenie/skidka-dok-stanciya-besprovodnaya-myshka-razer-viper-ultimate-cyberpunk-ID2ctHi.html</t>
+          <t>https://www.olx.uz/d/oz/obyavlenie/tp-link-archer-ax55-ax3000-dvuxdiapazonnyj-gigabitnyj-wifi-6-router-ID2IwvI.html</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>215 у.е.</t>
+          <t>85 у.е.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Toshkent, Yakkasaroy tumani - 26-avgust, 2022</t>
+          <t>Toshkent, Mirobod tumani - Bugunda 09:40</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>26-avgust, 2022</t>
+          <t>Bugunda 09:40</t>
         </is>
       </c>
     </row>
@@ -638,6 +638,1402 @@
       <c r="F7" t="inlineStr">
         <is>
           <t>Bugunda 13:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Wi-Fi роутер Xiaomi Mi Wi-Fi Router 4C</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/wi-fi-router-xiaomi-mi-wi-fi-router-4c-ID2H35f.html</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>390 000 so’m</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Toshkent, Yunusobod tumani - Bugunda 13:44</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Bugunda 13:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Printer Epson L355 цветной</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/printer-epson-l355-cvetnoj-ID2YjzA.html</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1 000 000 so’m</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Toshkent, Yunusobod tumani - Bugunda 13:40</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Bugunda 13:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>4G  WiFi router sim картаlik  LB-Link BL-CPE450H. УСТАНОВКА БЕСПЛАТНО!</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/4g-wifi-router-sim-kartalik-lb-link-bl-cpe450h-ustanovka-besplatno-ID2JEvN.html</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">45 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Buxoro - Bugunda 13:40</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Bugunda 13:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Wifi usilitel Tplink N300 TL-WA850RE Extender</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/wifi-usilitel-tplink-n300-tl-wa850re-extender-ID2YjyV.html</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">139 000 so’mKelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Toshkent, Chilonzor tumani - Bugunda 13:38</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Bugunda 13:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Принтер МФУ DocuCentre SC2020 (Перечислением)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/printer-mfu-docucentre-sc2020-perechisleniem-ID2WUrc.html</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">24 500 000 so’mKelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Toshkent, Yakkasaroy tumani - Bugunda 13:38</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Bugunda 13:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>LB-LINK WR450H Вайфай роутер/Точка доступа/Усилитель вай фай</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/lb-link-wr450h-vajfaj-router-tochka-dostupa-usilitel-vaj-faj-ID2JEy4.html</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">20 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Buxoro - Bugunda 13:35</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Bugunda 13:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Продается игровой руль  Logitech G27</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/prodaetsya-igrovoj-rul-logitech-g27-ID2Yjxw.html</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">300 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Olmaliq - Bugunda 13:34</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Bugunda 13:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Epson L850 Цветной Принтер</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/epson-l850-cvetnoj-printer-ID2XUcd.html</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4 000 000 so’m</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Nukus - 25-avgust, 2022</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>25-avgust, 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Восстановление печатающей головки Canon PF03/04/06</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/vosstanovlenie-pechatayushhej-golovki-canon-pf03-04-06-ID2OCKC.html</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2 300 000 so’m</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Toshkent, Shayxontohur tumani - 30-avgust, 2022</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>30-avgust, 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ITK Патч панель и комплектующие СКС</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/itk-patch-panel-i-komplektuyushhie-sks-ID1wx3V.html</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>10 000 so’m</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Toshkent, Yunusobod tumani - 30-avgust, 2022</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>30-avgust, 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Новый   VDSL/ADSL  wi-fi modem  роутер TP-Link VN020-F3</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/novyj-vdsl-adsl-wi-fi-modem-router-tp-link-vn020-f3-ID2PqRd.html</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">26 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Buxoro - Bugunda 13:32</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Bugunda 13:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Epson M1100 черно белый принтер с большим контейнером заправки</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/epson-m1100-cherno-belyj-printer-s-bolshim-kontejnerom-zapravki-ID2JEHg.html</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">185 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Buxoro - Bugunda 13:31</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Bugunda 13:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Новый принтер Epson L3101</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/novyj-printer-epson-l3101-ID2V2H7.html</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">195 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Buxoro - Bugunda 13:30</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Bugunda 13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Epson L3150 новый цветной принтер/ксерокс/сканер ТРИ В ОДНОМ + WIFI</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/epson-l3150-novyj-cvetnoj-printer-kseroks-skaner-tri-v-odnom-wifi-ID2V2IQ.html</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">215 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Buxoro - Bugunda 13:29</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Bugunda 13:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Новый принтер Epson M2120</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/novyj-printer-epson-m2120-ID2V27t.html</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">265 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Buxoro - Bugunda 13:28</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Bugunda 13:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Достовка безплатно! Метоо C20! Sifatli simsiz klaviatura  va Mishka</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/dostovka-bezplatno-metoo-c20-sifatli-simsiz-klaviatura-va-mishka-ID2rwsB.html</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>139 000 so’m</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Toshkent, Shayxontohur tumani - Bugunda 13:28</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Bugunda 13:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Акция! Доставка по Узбекистан  !Logitech C270 веб камера! web kamera!</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/akciya-dostavka-po-uzbekistan-logitech-c270-veb-kamera-web-kamera-ID2F6jo.html</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>29 у.е.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Toshkent, Yunusobod tumani - Bugunda 13:27</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Bugunda 13:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Принтер OKI C833dnl</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/printer-oki-c833dnl-ID2ShUb.html</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>30 000 000 so’m</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>To'ytepa - Bugunda 13:21</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Bugunda 13:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>kserokopiya 3а1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/kserokopiya-3a1-ID2Y2Kx.html</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1 100 000 so’m</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Samarqand - Bugunda 13:06</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Bugunda 13:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>принтер цветной epson tx650 копир сканер ксерокс 6 цветов</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/printer-cvetnoj-epson-tx650-kopir-skaner-kseroks-6-cvetov-ID2YjnW.html</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>1 400 000 so’m</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Toshkent, Yashnobod tumani - Bugunda 12:54</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Bugunda 12:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>canon mf 3010 sotiladi</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/canon-mf-3010-sotiladi-ID2Y2Ot.html</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>1 200 000 so’m</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Samarqand - 30-avgust, 2022</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>30-avgust, 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Новый! TP-Link Archer  AC1200 Двухдиапазонный Wi-Fi роутер.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/novyj-tp-link-archer-ac1200-dvuxdiapazonnyj-wi-fi-router-ID2l7yN.html</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>304 999 so’m</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Toshkent, Yunusobod tumani - Bugunda 09:48</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Bugunda 09:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Tp-link Deco E4 (2-pack) AC1200 Домашняя Mesh Wi-Fi система</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/tp-link-deco-e4-2-pack-ac1200-domashnyaya-mesh-wi-fi-sistema-ID2OQ5q.html</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>839 999 so’m</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Toshkent, Yakkasaroy tumani - 29-avgust, 2022</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>29-avgust, 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Epson L1800 printer</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/epson-l1800-printer-ID2VfO8.html</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 200 000 so’mKelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Buxoro - Bugunda 12:48</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Bugunda 12:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Canon 3010 3v1 sotiladi</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/canon-3010-3v1-sotiladi-ID2XL4S.html</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2 000 000 so’m</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Asaka - Bugunda 12:44</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Bugunda 12:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Проводная игровая мышь AULA F808 (Garantiya) (Tezkor Dostavka)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/provodnaya-igrovaya-mysh-aula-f808-garantiya-tezkor-dostavka-ID2ROcc.html</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>170 000 so’m</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Toshkent, Olmazor tumani - Bugunda 12:44</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Bugunda 12:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Canon  ir2016 a3 a4 есть 5 шт</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/canon-ir2016-a3-a4-est-5-sht-ID2OoMg.html</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">85 у.е.Kelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Toshkent, Yakkasaroy tumani - Bugunda 12:44</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Bugunda 12:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Роутер ADSL2+(TP-link: Model TD: W8901N)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/router-adsl2-tp-link-model-td-w8901n-ID2Yjlx.html</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>40 000 so’m</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Toshkent, Yakkasaroy tumani - Bugunda 12:44</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Bugunda 12:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Logitech G29 Спортивный руль на (PLS 3,4,5)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/logitech-g29-sportivnyj-rul-na-pls-3-4-5-ID2ysFP.html</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>4 400 000 so’m</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Toshkent, Yakkasaroy tumani - Bugunda 12:42</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Bugunda 12:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Bezpravadnoy mishka</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/bezpravadnoy-mishka-ID2Ul9G.html</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>70 000 so’m</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Toshkent, Mirzo-Ulug‘bek tumani - Bugunda 12:39</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Bugunda 12:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Canon  LBP 6030 Image Class Принетр</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/canon-lbp-6030-image-class-prinetr-ID2XUCC.html</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 000 000 so’mKelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Nukus - Bugunda 12:32</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Bugunda 12:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Продаётся вай фай</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/prodayotsya-vaj-faj-ID2YjhQ.html</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>50 000 so’m</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Olmaliq - Bugunda 12:31</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Bugunda 12:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>TP-LINK ADSL2+ Modem Router</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/tp-link-adsl2-modem-router-ID2y6kk.html</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>200 000 so’m</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Yangiyo'l - Bugunda 12:23</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Bugunda 12:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>СКИДКА до 05.09.22!Беспроводная мышка/мышь Glorious Model O Wireless</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/skidka-do-05-09-22-besprovodnaya-myshka-mysh-glorious-model-o-wireless-ID2pqWG.html</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>89 у.е.</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Toshkent, Yakkasaroy tumani - 26-avgust, 2022</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>26-avgust, 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Продам Wi-Fi роутер, с готовым интернетом (мобильный интернет)</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/prodam-wi-fi-router-s-gotovym-internetom-mobilnyj-internet-ID2FhLb.html</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>120 000 so’m</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Farg‘ona - 01-avgust, 2022</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>01-avgust, 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>TP-Link Deco E4 (2-pack) AC1200 Домашняя Mesh Wi-Fi система.</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/tp-link-deco-e4-2-pack-ac1200-domashnyaya-mesh-wi-fi-sistema-ID1JoAW.html</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">840 000 so’mKelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Toshkent, Mirzo-Ulug‘bek tumani - Bugunda 04:14</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Bugunda 04:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ZyXEL роутер модем</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/zyxel-router-modem-ID2UllQ.html</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>100 у.е.</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Samarqand - Bugunda 12:22</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Bugunda 12:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Сетевой LAN Кабель Original 40м</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/setevoj-lan-kabel-original-40m-ID2Wc26.html</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>85 000 so’m</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Toshkent, Shayxontohur tumani - Bugunda 12:19</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Bugunda 12:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>СРОЧНО!!! Продаётся 4G LTE MIFI Router</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/srochno-prodayotsya-4g-lte-mifi-router-ID2Yjew.html</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">400 000 so’mKelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Toshkent, Shayxontohur tumani - Bugunda 12:17</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Bugunda 12:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Принтер Canon MF443dw</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/printer-canon-mf443dw-ID2VfEC.html</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 200 000 so’mKelishilgan
+</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Samarqand - Bugunda 12:16</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Bugunda 12:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Tp link wi fi router 150mb 740</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/tp-link-wi-fi-router-150mb-740-ID2XPII.html</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>50 000 so’m</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Toshkent, Yashnobod tumani - Bugunda 12:12</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Bugunda 12:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>продам новый беспроводной клавиатура и мышь Defender C775/С ДОСТАВКОЙ</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/prodam-novyj-besprovodnoj-klaviatura-i-mysh-defender-c775-s-dostavkoj-ID2PiJd.html</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>210 000 so’m</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Toshkent, Yunusobod tumani - Bugunda 12:07</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Bugunda 12:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Продается новый Magic Mouse 2 (белого цвета)</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/prodaetsya-novyj-magic-mouse-2-belogo-cveta-ID2WEWT.html</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>65 у.е.</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Toshkent, Mirzo-Ulug‘bek tumani - Bugunda 12:03</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Bugunda 12:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>HUAWEI Wi-Fi poytor</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/huawei-wi-fi-poytor-ID2VfA2.html</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>50 000 so’m</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Qarshi - Bugunda 12:02</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Bugunda 12:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Струйный Принтер Canon PIXMA G2020</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/strujnyj-printer-canon-pixma-g2020-ID2QkxT.html</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>210 у.е.</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Toshkent, Sirg‘ali tumani - Bugunda 12:00</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Bugunda 12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Wi-fi роутеры,машуртизатор</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://www.olx.uz/d/oz/obyavlenie/wi-fi-routery-mashurtizator-ID2Yj96.html</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>200 000 so’m</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Toshkent, Mirobod tumani - Bugunda 11:57</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Bugunda 11:57</t>
         </is>
       </c>
     </row>

</xml_diff>